<commit_message>
ELI-114: fixing fixture script data that I think can lead to occasional test failures because it is invalid with respect to validation rules
see https://travis-ci.org/incodehq/contactapp/builds/122047183, for example
</commit_message>
<xml_diff>
--- a/backend/fixture/src/main/java/org/incode/eurocommercial/contactapp/fixture/scenarios/demo/DemoFixture.xlsx
+++ b/backend/fixture/src/main/java/org/incode/eurocommercial/contactapp/fixture/scenarios/demo/DemoFixture.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvanderwal/src/github/incodehq/contactapp/backend/fixture/src/main/java/domainapp/fixture/scenarios/demo/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1800" yWindow="-25720" windowWidth="34620" windowHeight="16660"/>
+    <workbookView xWindow="-1800" yWindow="-25725" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="ContactImport" sheetId="5" r:id="rId1"/>
@@ -98,42 +93,18 @@
     <t>Bill Smith</t>
   </si>
   <si>
-    <t>+44 (0)20 111 2222</t>
-  </si>
-  <si>
-    <t>+44 (0)7770 222 123</t>
-  </si>
-  <si>
-    <t>+44 (0)1233 444 555</t>
-  </si>
-  <si>
     <t>bill.smith@acmecompany.com</t>
   </si>
   <si>
     <t>Bob Mills</t>
   </si>
   <si>
-    <t>+31 (0)20 999 1111</t>
-  </si>
-  <si>
-    <t>+31 (0)6 4444 3333</t>
-  </si>
-  <si>
     <t>bob.mills@acmecompany.com</t>
   </si>
   <si>
     <t>Mike Jones</t>
   </si>
   <si>
-    <t>+44 (0)20 7777 3333</t>
-  </si>
-  <si>
-    <t>+44 (0)7770 222 111</t>
-  </si>
-  <si>
-    <t>+44 (0)1892 999 222</t>
-  </si>
-  <si>
     <t>mike.jones@acmecompany.com</t>
   </si>
   <si>
@@ -143,42 +114,24 @@
     <t>EuroCope Amsterdam</t>
   </si>
   <si>
-    <t>+31(0)20-555 1000</t>
-  </si>
-  <si>
     <t>info@xyz.nl</t>
   </si>
   <si>
     <t>Anne van Hope</t>
   </si>
   <si>
-    <t>+31 (0)20 222 1234</t>
-  </si>
-  <si>
     <t>annvanhope@eurocope.com</t>
   </si>
   <si>
     <t>Leo Gardener</t>
   </si>
   <si>
-    <t>+31 (0)20 456 7891</t>
-  </si>
-  <si>
-    <t>+31 (0) 6 432 1234</t>
-  </si>
-  <si>
     <t>leo.gardener@kramer-kramer.com</t>
   </si>
   <si>
     <t>David Goodhew</t>
   </si>
   <si>
-    <t>+31 (0)20 444 1234</t>
-  </si>
-  <si>
-    <t>+31 (0) 6 112 2334</t>
-  </si>
-  <si>
     <t>d.goodnew@abcdef.nl</t>
   </si>
   <si>
@@ -267,6 +220,48 @@
   </si>
   <si>
     <t>Amiens Property</t>
+  </si>
+  <si>
+    <t>+44 20 111 2222</t>
+  </si>
+  <si>
+    <t>+44 7770 222 123</t>
+  </si>
+  <si>
+    <t>+44 1233 444 555</t>
+  </si>
+  <si>
+    <t>+31 20 999 1111</t>
+  </si>
+  <si>
+    <t>+44 20 7777 3333</t>
+  </si>
+  <si>
+    <t>+31 20-555 1000</t>
+  </si>
+  <si>
+    <t>+31 20 222 1234</t>
+  </si>
+  <si>
+    <t>+31 20 456 7891</t>
+  </si>
+  <si>
+    <t>+31 20 444 1234</t>
+  </si>
+  <si>
+    <t>+31 6 112 2334</t>
+  </si>
+  <si>
+    <t>+31 6 432 1234</t>
+  </si>
+  <si>
+    <t>+44 7770 222 111</t>
+  </si>
+  <si>
+    <t>+31 6 4444 3333</t>
+  </si>
+  <si>
+    <t>+44 1892 999 222</t>
   </si>
 </sst>
 </file>
@@ -728,18 +723,18 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -776,70 +771,70 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -848,32 +843,32 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="11" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>7</v>
@@ -884,32 +879,32 @@
         <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="12" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="10" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -917,31 +912,31 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="14" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
@@ -951,26 +946,26 @@
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="15" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="13" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>15</v>
@@ -978,41 +973,41 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="7" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="15" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="15" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>17</v>
@@ -1020,13 +1015,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1040,21 +1035,21 @@
         <v>20</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="16" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ELI-134: fixing bad test data causing random failure in CI
</commit_message>
<xml_diff>
--- a/backend/fixture/src/main/java/org/incode/eurocommercial/contactapp/fixture/scenarios/demo/DemoFixture.xlsx
+++ b/backend/fixture/src/main/java/org/incode/eurocommercial/contactapp/fixture/scenarios/demo/DemoFixture.xlsx
@@ -237,9 +237,6 @@
     <t>+44 20 7777 3333</t>
   </si>
   <si>
-    <t>+31 20-555 1000</t>
-  </si>
-  <si>
     <t>+31 20 222 1234</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>+44 1892 999 222</t>
+  </si>
+  <si>
+    <t>+31 20 555 1000</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
         <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="10" t="s">
@@ -828,10 +828,10 @@
         <v>71</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>28</v>
@@ -847,7 +847,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="11" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -863,7 +863,7 @@
         <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -882,10 +882,10 @@
         <v>34</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="12" t="s">
@@ -897,10 +897,10 @@
         <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="10" t="s">

</xml_diff>